<commit_message>
dummy candidate list changes
</commit_message>
<xml_diff>
--- a/lib/candidates.xlsx
+++ b/lib/candidates.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>name</t>
   </si>
@@ -118,58 +118,91 @@
     <t>9846284959</t>
   </si>
   <si>
-    <t>james@example.com</t>
+    <t>Smith James</t>
+  </si>
+  <si>
+    <t>smithjames@example.com</t>
   </si>
   <si>
     <t>9846284960</t>
   </si>
   <si>
-    <t>micheal@example.com</t>
+    <t>Smith Michael</t>
+  </si>
+  <si>
+    <t>smithmicheal@example.com</t>
   </si>
   <si>
     <t>9846284961</t>
   </si>
   <si>
+    <t>Johnson James</t>
+  </si>
+  <si>
+    <t>johnsonjames@example.com</t>
+  </si>
+  <si>
     <t>9846284962</t>
   </si>
   <si>
-    <t>robert@example.com</t>
+    <t>Smith Robert</t>
+  </si>
+  <si>
+    <t>smithrobert@example.com</t>
   </si>
   <si>
     <t>9846284963</t>
   </si>
   <si>
-    <t>maria@example.com</t>
+    <t>Garcia Maria</t>
+  </si>
+  <si>
+    <t>garciamaria@example.com</t>
   </si>
   <si>
     <t>9846284964</t>
   </si>
   <si>
-    <t>david@example.com</t>
+    <t>Smith David</t>
+  </si>
+  <si>
+    <t>smithdavid@example.com</t>
   </si>
   <si>
     <t>9846284965</t>
   </si>
   <si>
-    <t>rodrigues@example.com</t>
+    <t>Rodriguez Maria</t>
+  </si>
+  <si>
+    <t>rodriguezmaria@example.com</t>
   </si>
   <si>
     <t>9846284966</t>
   </si>
   <si>
-    <t>mary@example.com</t>
+    <t>Smith Mary</t>
+  </si>
+  <si>
+    <t>smithmary@example.com</t>
   </si>
   <si>
     <t>9846284967</t>
   </si>
   <si>
-    <t>hernandez@example.com</t>
+    <t>Hernandez Maria</t>
+  </si>
+  <si>
+    <t>hernandezmaria@example.com</t>
   </si>
   <si>
     <t>9846284968</t>
   </si>
   <si>
-    <t>martinez@example.com</t>
+    <t>Martinez Maria</t>
+  </si>
+  <si>
+    <t>martinezmaria@example.com</t>
   </si>
   <si>
     <t>9846284969</t>
@@ -264,7 +297,9 @@
     <xf borderId="0" fillId="3" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -811,14 +846,14 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>7</v>
@@ -840,14 +875,14 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>37</v>
+      <c r="A13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>7</v>
@@ -869,14 +904,14 @@
       <c r="S13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>35</v>
+      <c r="A14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>7</v>
@@ -898,14 +933,14 @@
       <c r="S14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>40</v>
+      <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>7</v>
@@ -927,14 +962,14 @@
       <c r="S15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>42</v>
+      <c r="A16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>7</v>
@@ -956,14 +991,14 @@
       <c r="S16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>44</v>
+      <c r="A17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>7</v>
@@ -985,14 +1020,14 @@
       <c r="S17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>23</v>
+      <c r="A18" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>7</v>
@@ -1014,14 +1049,14 @@
       <c r="S18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>48</v>
+      <c r="A19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>7</v>
@@ -1043,14 +1078,14 @@
       <c r="S19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>29</v>
+      <c r="A20" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>7</v>
@@ -1072,14 +1107,14 @@
       <c r="S20" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>32</v>
+      <c r="A21" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>7</v>

</xml_diff>